<commit_message>
Update table Sszw (#1768)
* UPdate sszw

* Fill Delay Cell generic

* update

* Update excel template

* resolve conflict

* Format xtend

* Update java/bundles/org.eclipse.set.feature.table.pt1/src/org/eclipse/set/feature/table/pt1/sszw/SszwTransformator.xtend

Co-authored-by: Marius Heine <m.heine@geprog.com>

* Update table reference

---------

Co-authored-by: Marius Heine <m.heine@geprog.com>
Co-authored-by: eclipse-set-bot <set-bot@eclipse.org>
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sszw_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sszw_vorlage.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SB\set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C9168-F4EA-47A8-85D4-BF5A3600E26F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A943E7-744B-4743-B996-935D1C184D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="28800" windowHeight="11625" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sszw_Beispielbefüllung" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>A</t>
   </si>
@@ -107,12 +107,6 @@
     <t>Weiche</t>
   </si>
   <si>
-    <t>Links (KrW: A abzw.)</t>
-  </si>
-  <si>
-    <t>Rechts (KrW: B abzw.)</t>
-  </si>
-  <si>
     <t>km/h</t>
   </si>
   <si>
@@ -126,6 +120,16 @@
   </si>
   <si>
     <t>Ansteuerung</t>
+  </si>
+  <si>
+    <t>Grundform</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>keine Übertrag.
+an RBC</t>
   </si>
 </sst>
 </file>
@@ -165,7 +169,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -175,19 +179,6 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -480,138 +471,120 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -701,9 +674,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -741,9 +714,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -776,26 +749,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -828,26 +784,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1021,220 +960,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K35" sqref="K35"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="10.15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="20" customWidth="1"/>
-    <col min="7" max="12" width="11.42578125" style="20" customWidth="1"/>
-    <col min="13" max="14" width="13.28515625" style="20" customWidth="1"/>
-    <col min="15" max="15" width="48.7109375" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="20"/>
+    <col min="1" max="1" width="3.28515625" style="16" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" style="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="16" customWidth="1"/>
+    <col min="7" max="12" width="11.42578125" style="16" customWidth="1"/>
+    <col min="13" max="14" width="13.28515625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="11" style="20" customWidth="1"/>
+    <col min="16" max="16" width="45.42578125" style="16" customWidth="1"/>
+    <col min="17" max="16384" width="11.28515625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="15"/>
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="12" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="13" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="13" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="1:16" s="1" customFormat="1" ht="11.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="37" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="38"/>
-      <c r="O2" s="18" t="s">
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="30"/>
+      <c r="O2" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:16" s="1" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="35"/>
+      <c r="I3" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" s="35"/>
+      <c r="M3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="38"/>
+      <c r="P3" s="17"/>
+    </row>
+    <row r="4" spans="1:16" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="36" t="s">
+      <c r="D4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" s="43"/>
-      <c r="M3" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="21"/>
+      <c r="E4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="18"/>
+      <c r="P4" s="18"/>
     </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="6" t="s">
+    <row r="5" spans="1:16" s="1" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="6"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="22"/>
+      <c r="J5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="19"/>
+      <c r="P5" s="19"/>
     </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="23"/>
+    <row r="6" spans="1:16" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="24"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="21"/>
     </row>
-    <row r="6" spans="1:15" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="25"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="30"/>
-    </row>
-    <row r="7" spans="1:15" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="34"/>
-      <c r="O7" s="35"/>
+    <row r="7" spans="1:16" ht="10.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="B2:H2"/>
     <mergeCell ref="E3:F3"/>
@@ -1242,6 +1193,7 @@
     <mergeCell ref="I2:L2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.19685039370078741" bottom="1.3779527559055118" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
@@ -1250,6 +1202,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1441,19 +1406,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
@@ -1501,6 +1453,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52AA9053-CA78-458B-BFEC-B0A103F9F68C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B642628-E0AC-4F61-AC13-56E3126AE48A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1519,22 +1487,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DF743650-405A-4EB5-9BE5-79180E38FBC9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52AA9053-CA78-458B-BFEC-B0A103F9F68C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9CFCEAE-5A31-4E8D-871E-0FEB90E546B0}">
   <ds:schemaRefs>

</xml_diff>